<commit_message>
added data summary and spreadsheet labels
</commit_message>
<xml_diff>
--- a/Sort_keys.xlsx
+++ b/Sort_keys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fanwu/Documents/Impedance_sort/Impedance_sort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB61C6A-41CF-8143-BF56-27511C66D43E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A425453-B379-434F-894B-EE7F689BBB0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="980" windowWidth="27640" windowHeight="15580" xr2:uid="{AC2DE5D7-96A3-1447-9F5B-30952FFE315D}"/>
+    <workbookView xWindow="1160" yWindow="980" windowWidth="27640" windowHeight="15580" xr2:uid="{AC2DE5D7-96A3-1447-9F5B-30952FFE315D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,43 +36,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>ASSY156</t>
-  </si>
-  <si>
-    <t>ASSY116</t>
-  </si>
-  <si>
-    <t>ASSY236</t>
-  </si>
-  <si>
     <t>NanoZ</t>
   </si>
   <si>
-    <t>ASSY77</t>
+    <t>ASSY-1</t>
   </si>
   <si>
-    <t>ASSY158A</t>
+    <t>ASSY-37</t>
   </si>
   <si>
-    <t>ASSY158B</t>
+    <t>ASSY-77</t>
   </si>
   <si>
-    <t>ASSY196</t>
+    <t>ASSY-79</t>
   </si>
   <si>
-    <t>ASSY276</t>
+    <t>ASSY-116</t>
   </si>
   <si>
-    <t>ASSY316</t>
+    <t>ASSY-156</t>
   </si>
   <si>
-    <t>ASSY37</t>
+    <t>ASSY-158A</t>
   </si>
   <si>
-    <t>ASSY1</t>
+    <t>ASSY-158B</t>
   </si>
   <si>
-    <t>ASSY79</t>
+    <t>ASSY-196</t>
+  </si>
+  <si>
+    <t>ASSY-236</t>
+  </si>
+  <si>
+    <t>ASSY-276</t>
+  </si>
+  <si>
+    <t>ASSY-316</t>
   </si>
 </sst>
 </file>
@@ -633,7 +633,7 @@
   <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,43 +644,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="M1" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -695,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <f>A2</f>
+        <f t="shared" ref="D2:D33" si="0">A2</f>
         <v>1</v>
       </c>
       <c r="E2" s="3">
@@ -740,7 +740,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <f>A3</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E3" s="6">
@@ -773,19 +773,19 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f t="shared" ref="A4:C65" si="0">A3+1</f>
+        <f t="shared" ref="A4:C65" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D4">
-        <f>A4</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E4" s="8">
@@ -818,19 +818,19 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="D5">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E5" s="5">
@@ -863,19 +863,19 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="D6">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E6" s="5">
@@ -908,19 +908,19 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D7">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E7" s="8">
@@ -953,19 +953,19 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="D8">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E8" s="8">
@@ -998,19 +998,19 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="D9">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E9" s="8">
@@ -1043,15 +1043,15 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="D10">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E10" s="5">
@@ -1084,15 +1084,15 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="D11">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E11" s="8">
@@ -1125,15 +1125,15 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="D12">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="E12" s="8">
@@ -1166,15 +1166,15 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="D13">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E13" s="8">
@@ -1207,15 +1207,15 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="D14">
-        <f>A14</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="E14" s="5">
@@ -1248,15 +1248,15 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="D15">
-        <f>A15</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="E15" s="5">
@@ -1289,15 +1289,15 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="D16">
-        <f>A16</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="E16" s="5">
@@ -1330,15 +1330,15 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="D17">
-        <f>A17</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="E17" s="5">
@@ -1371,15 +1371,15 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="D18">
-        <f>A18</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="E18" s="5">
@@ -1412,15 +1412,15 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="D19">
-        <f>A19</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="E19" s="5">
@@ -1453,15 +1453,15 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="D20">
-        <f>A20</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="E20" s="5">
@@ -1494,15 +1494,15 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="D21">
-        <f>A21</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="E21" s="5">
@@ -1535,15 +1535,15 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="D22">
-        <f>A22</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="E22" s="8">
@@ -1576,15 +1576,15 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="D23">
-        <f>A23</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="E23" s="8">
@@ -1617,15 +1617,15 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="D24">
-        <f>A24</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="E24" s="8">
@@ -1658,15 +1658,15 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="D25">
-        <f>A25</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="E25" s="5">
@@ -1699,19 +1699,19 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26:B31" si="1">B27-1</f>
+        <f t="shared" ref="B26:B31" si="2">B27-1</f>
         <v>9</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="D26">
-        <f>A26</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="E26" s="8">
@@ -1744,19 +1744,19 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="D27">
-        <f>A27</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="E27" s="5">
@@ -1789,19 +1789,19 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="D28">
-        <f>A28</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="E28" s="8">
@@ -1834,19 +1834,19 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="D29">
-        <f>A29</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="E29" s="5">
@@ -1879,19 +1879,19 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="D30">
-        <f>A30</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E30" s="8">
@@ -1924,19 +1924,19 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="D31">
-        <f>A31</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="E31" s="5">
@@ -1969,7 +1969,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B32">
@@ -1977,11 +1977,11 @@
         <v>15</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="D32">
-        <f>A32</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="E32" s="8">
@@ -2014,18 +2014,18 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B33">
         <v>16</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="D33">
-        <f>A33</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="E33" s="8">
@@ -2058,11 +2058,11 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="D34">
-        <f>A34</f>
+        <f t="shared" ref="D34:D65" si="3">A34</f>
         <v>33</v>
       </c>
       <c r="G34">
@@ -2080,11 +2080,11 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="D35">
-        <f>A35</f>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="G35">
@@ -2102,11 +2102,11 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="D36">
-        <f>A36</f>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="G36">
@@ -2124,11 +2124,11 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="D37">
-        <f>A37</f>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="G37">
@@ -2146,11 +2146,11 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="D38">
-        <f>A38</f>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="G38">
@@ -2168,11 +2168,11 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="D39">
-        <f>A39</f>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="G39">
@@ -2190,11 +2190,11 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="D40">
-        <f>A40</f>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="G40">
@@ -2212,11 +2212,11 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="D41">
-        <f>A41</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="G41">
@@ -2234,11 +2234,11 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="D42">
-        <f>A42</f>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="G42">
@@ -2256,11 +2256,11 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="D43">
-        <f>A43</f>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="G43">
@@ -2278,11 +2278,11 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="D44">
-        <f>A44</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="G44">
@@ -2300,11 +2300,11 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="D45">
-        <f>A45</f>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="G45">
@@ -2322,11 +2322,11 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="D46">
-        <f>A46</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="G46">
@@ -2344,11 +2344,11 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="D47">
-        <f>A47</f>
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="G47">
@@ -2366,11 +2366,11 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="D48">
-        <f>A48</f>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="G48">
@@ -2388,11 +2388,11 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="D49">
-        <f>A49</f>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="G49">
@@ -2410,11 +2410,11 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="D50">
-        <f>A50</f>
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
       <c r="G50">
@@ -2432,11 +2432,11 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="D51">
-        <f>A51</f>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="G51">
@@ -2454,11 +2454,11 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="D52">
-        <f>A52</f>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
       <c r="G52">
@@ -2476,11 +2476,11 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="D53">
-        <f>A53</f>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="G53">
@@ -2498,11 +2498,11 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="D54">
-        <f>A54</f>
+        <f t="shared" si="3"/>
         <v>53</v>
       </c>
       <c r="G54">
@@ -2520,11 +2520,11 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="D55">
-        <f>A55</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="G55">
@@ -2542,11 +2542,11 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="D56">
-        <f>A56</f>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="G56">
@@ -2564,11 +2564,11 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="D57">
-        <f>A57</f>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="G57">
@@ -2586,11 +2586,11 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="D58">
-        <f>A58</f>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="G58">
@@ -2608,11 +2608,11 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="D59">
-        <f>A59</f>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
       <c r="G59">
@@ -2630,11 +2630,11 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="D60">
-        <f>A60</f>
+        <f t="shared" si="3"/>
         <v>59</v>
       </c>
       <c r="G60">
@@ -2652,11 +2652,11 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="D61">
-        <f>A61</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="G61">
@@ -2674,11 +2674,11 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="D62">
-        <f>A62</f>
+        <f t="shared" si="3"/>
         <v>61</v>
       </c>
       <c r="G62">
@@ -2696,11 +2696,11 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="D63">
-        <f>A63</f>
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
       <c r="G63">
@@ -2718,11 +2718,11 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="D64">
-        <f>A64</f>
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
       <c r="G64">
@@ -2740,11 +2740,11 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="D65">
-        <f>A65</f>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="G65">

</xml_diff>